<commit_message>
start and end times added
Change to allow Group Start and End times
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t xml:space="preserve">Guide to using the SiteWorks import templates</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t xml:space="preserve">When</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End time</t>
   </si>
   <si>
     <t xml:space="preserve">Venue</t>
@@ -425,36 +431,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -531,13 +541,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -816,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -828,29 +838,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -866,7 +876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -878,36 +888,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -923,63 +933,69 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>74</v>
+      <c r="P1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -994,7 +1010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1007,35 +1023,35 @@
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>79</v>
+      <c r="J1" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1032 alter group status term Suspended to Dormant
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">Wait list only</t>
   </si>
   <si>
-    <t xml:space="preserve">Suspended</t>
+    <t xml:space="preserve">Dormant</t>
   </si>
   <si>
     <t xml:space="preserve">Closed</t>
@@ -541,14 +541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -826,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -836,7 +836,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
@@ -876,7 +876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -886,7 +886,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
@@ -933,17 +933,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1010,7 +1010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1020,7 +1020,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">

</xml_diff>

<commit_message>
Add 'End time' to spreadsheet template for Events
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
   <si>
     <t xml:space="preserve">Guide to using the SiteWorks import templates</t>
   </si>
@@ -547,7 +547,7 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +836,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
@@ -886,7 +886,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
@@ -943,7 +943,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1014,13 +1014,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1036,21 +1036,24 @@
         <v>65</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update instructions in spreadsheet
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -119,7 +119,8 @@
     <t xml:space="preserve">The ‘Status’ must be one of the terms shown in the list below.  You can use either the full or the short form.</t>
   </si>
   <si>
-    <t xml:space="preserve">The ‘Category’ must be an existing group category.  Create new group categories if necessary before importing groups that refer to them. The column heading 'Category' must be used even if you have selected another term to be used on your website.</t>
+    <t xml:space="preserve">The ‘Category’ must be an existing group category.  Create new group categories if necessary before importing groups that refer to them. The column heading 'Category' must be used even if you have selected another term to be used on your website.
+Multiple group categories should be separated using the vertical bar character |,  for example ‘History|Virtual’.</t>
   </si>
   <si>
     <t xml:space="preserve">The ‘Day’ must be one of  'Monday', 'Tuesday', 'Wednesday', 'Thursday', 'Friday', 'Saturday', 'Sunday' or may be omitted.</t>
@@ -547,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -677,7 +678,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="32.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="42.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
@@ -836,7 +837,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
@@ -886,7 +887,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
@@ -943,7 +944,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1016,11 +1017,11 @@
   </sheetPr>
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">

</xml_diff>

<commit_message>
change group status short text "Waiting list" in spreadsheet template
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -216,7 +216,7 @@
     <t xml:space="preserve">Full</t>
   </si>
   <si>
-    <t xml:space="preserve">Wait list only</t>
+    <t xml:space="preserve">Waiting list</t>
   </si>
   <si>
     <t xml:space="preserve">Dormant</t>
@@ -548,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -837,7 +837,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
@@ -887,7 +887,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
@@ -944,7 +944,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1021,7 +1021,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">

</xml_diff>

<commit_message>
update version, readme, help text
</commit_message>
<xml_diff>
--- a/assets/importtemplate.xlsx
+++ b/assets/importtemplate.xlsx
@@ -77,7 +77,7 @@
     <t xml:space="preserve">Please refer to the SiteWorks documentation for a full guide to using the CSV import / export facility</t>
   </si>
   <si>
-    <t xml:space="preserve">It is highly recommended that you have a backup of your website before importing from your CSV files.</t>
+    <t xml:space="preserve">It is highly recommended that you ensure your website is backed up before importing from your CSV files.</t>
   </si>
   <si>
     <t xml:space="preserve">Notes on the content of import files</t>
@@ -144,7 +144,7 @@
     <t xml:space="preserve">The columns ‘Name’, ‘Category’ and ‘Date’ are required.  All other columns are optional and may be omitted.</t>
   </si>
   <si>
-    <t xml:space="preserve">The ‘Category’ must be an existing event category.  Create new event categories if necessary before importing events that refer to them.</t>
+    <t xml:space="preserve">The ‘Category’ must be an existing event category.  Create new event categories if necessary before importing events that refer to them.  Multiple event categories should be separated using the vertical bar character |,  for example ‘Meeting|Social’.</t>
   </si>
   <si>
     <r>
@@ -548,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -837,7 +837,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="16"/>
   </cols>
@@ -887,7 +887,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="16.22"/>
@@ -944,7 +944,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
@@ -1021,7 +1021,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">

</xml_diff>